<commit_message>
all changes made and all formatting good
</commit_message>
<xml_diff>
--- a/Outputs/ICB_template.xlsx
+++ b/Outputs/ICB_template.xlsx
@@ -936,7 +936,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
     <col width="9.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="2.7109375" customWidth="1" style="20" min="2" max="2"/>
@@ -1142,7 +1142,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col width="9.140625" customWidth="1" style="33" min="1" max="1"/>
     <col width="11.140625" customWidth="1" style="34" min="2" max="3"/>
@@ -1642,7 +1642,7 @@
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="14.25" outlineLevelRow="2"/>
   <cols>
     <col width="9.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="15.85546875" customWidth="1" style="1" min="2" max="2"/>
@@ -23181,7 +23181,7 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="14.25" outlineLevelRow="1"/>
   <cols>
     <col width="9.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="15.85546875" customWidth="1" style="1" min="2" max="2"/>
@@ -40733,7 +40733,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="14.25" outlineLevelRow="1"/>
   <cols>
     <col width="9.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="15.85546875" customWidth="1" style="1" min="2" max="2"/>
@@ -58295,7 +58295,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="14.25" outlineLevelRow="1"/>
   <cols>
     <col width="9.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="15.85546875" customWidth="1" style="1" min="2" max="2"/>
@@ -58513,187 +58513,187 @@
       </c>
       <c r="D15" s="64" t="inlineStr">
         <is>
-          <t>2022-04-01</t>
+          <t>Apr-2022</t>
         </is>
       </c>
       <c r="E15" s="64" t="inlineStr">
         <is>
-          <t>2022-05-01</t>
+          <t>May-2022</t>
         </is>
       </c>
       <c r="F15" s="64" t="inlineStr">
         <is>
-          <t>2022-06-01</t>
+          <t>Jun-2022</t>
         </is>
       </c>
       <c r="G15" s="64" t="inlineStr">
         <is>
-          <t>2022-07-01</t>
+          <t>Jul-2022</t>
         </is>
       </c>
       <c r="H15" s="64" t="inlineStr">
         <is>
-          <t>2022-08-01</t>
+          <t>Aug-2022</t>
         </is>
       </c>
       <c r="I15" s="64" t="inlineStr">
         <is>
-          <t>2022-09-01</t>
+          <t>Sep-2022</t>
         </is>
       </c>
       <c r="J15" s="64" t="inlineStr">
         <is>
-          <t>2022-10-01</t>
+          <t>Oct-2022</t>
         </is>
       </c>
       <c r="K15" s="64" t="inlineStr">
         <is>
-          <t>2022-11-01</t>
+          <t>Nov-2022</t>
         </is>
       </c>
       <c r="L15" s="64" t="inlineStr">
         <is>
-          <t>2022-12-01</t>
+          <t>Dec-2022</t>
         </is>
       </c>
       <c r="M15" s="64" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>Jan-2023</t>
         </is>
       </c>
       <c r="N15" s="64" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>Feb-2023</t>
         </is>
       </c>
       <c r="O15" s="64" t="inlineStr">
         <is>
-          <t>2023-03-01</t>
+          <t>Mar-2023</t>
         </is>
       </c>
       <c r="P15" s="64" t="inlineStr">
         <is>
-          <t>2023-04-01</t>
+          <t>Apr-2023</t>
         </is>
       </c>
       <c r="Q15" s="64" t="inlineStr">
         <is>
-          <t>2023-05-01</t>
+          <t>May-2023</t>
         </is>
       </c>
       <c r="R15" s="64" t="inlineStr">
         <is>
-          <t>2023-06-01</t>
+          <t>Jun-2023</t>
         </is>
       </c>
       <c r="S15" s="64" t="inlineStr">
         <is>
-          <t>2023-07-01</t>
+          <t>Jul-2023</t>
         </is>
       </c>
       <c r="T15" s="64" t="inlineStr">
         <is>
-          <t>2023-08-01</t>
+          <t>Aug-2023</t>
         </is>
       </c>
       <c r="U15" s="64" t="inlineStr">
         <is>
-          <t>2023-09-01</t>
+          <t>Sep-2023</t>
         </is>
       </c>
       <c r="V15" s="64" t="inlineStr">
         <is>
-          <t>2023-10-01</t>
+          <t>Oct-2023</t>
         </is>
       </c>
       <c r="W15" s="64" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>Nov-2023</t>
         </is>
       </c>
       <c r="X15" s="64" t="inlineStr">
         <is>
-          <t>2023-12-01</t>
+          <t>Dec-2023</t>
         </is>
       </c>
       <c r="Y15" s="64" t="inlineStr">
         <is>
-          <t>2024-01-01</t>
+          <t>Jan-2024</t>
         </is>
       </c>
       <c r="Z15" s="64" t="inlineStr">
         <is>
-          <t>2024-02-01</t>
+          <t>Feb-2024</t>
         </is>
       </c>
       <c r="AA15" s="64" t="inlineStr">
         <is>
-          <t>2024-03-01</t>
+          <t>Mar-2024</t>
         </is>
       </c>
       <c r="AB15" s="64" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>Apr-2024</t>
         </is>
       </c>
       <c r="AC15" s="64" t="inlineStr">
         <is>
-          <t>2024-05-01</t>
+          <t>May-2024</t>
         </is>
       </c>
       <c r="AD15" s="64" t="inlineStr">
         <is>
-          <t>2024-06-01</t>
+          <t>Jun-2024</t>
         </is>
       </c>
       <c r="AE15" s="64" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>Jul-2024</t>
         </is>
       </c>
       <c r="AF15" s="64" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>Aug-2024</t>
         </is>
       </c>
       <c r="AG15" s="64" t="inlineStr">
         <is>
-          <t>2024-09-01</t>
+          <t>Sep-2024</t>
         </is>
       </c>
       <c r="AH15" s="64" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>Oct-2024</t>
         </is>
       </c>
       <c r="AI15" s="64" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>Nov-2024</t>
         </is>
       </c>
       <c r="AJ15" s="64" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>Dec-2024</t>
         </is>
       </c>
       <c r="AK15" s="64" t="inlineStr">
         <is>
-          <t>2025-01-01</t>
+          <t>Jan-2025</t>
         </is>
       </c>
       <c r="AL15" s="64" t="inlineStr">
         <is>
-          <t>2025-02-01</t>
+          <t>Feb-2025</t>
         </is>
       </c>
       <c r="AM15" s="64" t="inlineStr">
         <is>
-          <t>2025-03-01</t>
+          <t>Mar-2025</t>
         </is>
       </c>
       <c r="AN15" s="64" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>Apr-2025</t>
         </is>
       </c>
     </row>
@@ -59923,18 +59923,19 @@
       <c r="AJ25" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK25" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL25" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM25" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN25" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK25" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL25" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM25" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN25" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO25" s="90" t="n"/>
     </row>
     <row r="26" outlineLevel="1">
       <c r="B26" s="4" t="inlineStr">
@@ -60046,18 +60047,19 @@
       <c r="AJ26" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK26" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL26" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM26" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN26" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK26" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL26" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN26" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO26" s="90" t="n"/>
     </row>
     <row r="27" outlineLevel="1">
       <c r="B27" s="4" t="inlineStr">
@@ -60169,18 +60171,19 @@
       <c r="AJ27" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK27" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL27" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM27" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN27" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK27" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL27" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM27" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN27" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO27" s="90" t="n"/>
     </row>
     <row r="28" outlineLevel="1">
       <c r="B28" s="4" t="inlineStr">
@@ -60292,18 +60295,19 @@
       <c r="AJ28" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN28" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK28" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL28" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM28" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN28" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO28" s="90" t="n"/>
     </row>
     <row r="29" outlineLevel="1">
       <c r="B29" s="4" t="inlineStr">
@@ -60415,18 +60419,19 @@
       <c r="AJ29" s="86" t="n">
         <v>520</v>
       </c>
-      <c r="AK29" s="3" t="n">
+      <c r="AK29" s="86" t="n">
         <v>574</v>
       </c>
-      <c r="AL29" s="3" t="n">
+      <c r="AL29" s="86" t="n">
         <v>472</v>
       </c>
-      <c r="AM29" s="3" t="n">
+      <c r="AM29" s="86" t="n">
         <v>515</v>
       </c>
-      <c r="AN29" s="3" t="n">
+      <c r="AN29" s="86" t="n">
         <v>437</v>
       </c>
+      <c r="AO29" s="90" t="n"/>
     </row>
     <row r="30" outlineLevel="1">
       <c r="B30" s="4" t="inlineStr">
@@ -60538,18 +60543,19 @@
       <c r="AJ30" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK30" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL30" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM30" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN30" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK30" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM30" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN30" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO30" s="90" t="n"/>
     </row>
     <row r="31" outlineLevel="1">
       <c r="B31" s="4" t="inlineStr">
@@ -60661,18 +60667,19 @@
       <c r="AJ31" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK31" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL31" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM31" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN31" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK31" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL31" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM31" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN31" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO31" s="90" t="n"/>
     </row>
     <row r="32" outlineLevel="1">
       <c r="B32" s="4" t="inlineStr">
@@ -60784,18 +60791,19 @@
       <c r="AJ32" s="86" t="n">
         <v>1170</v>
       </c>
-      <c r="AK32" s="3" t="n">
+      <c r="AK32" s="86" t="n">
         <v>1342</v>
       </c>
-      <c r="AL32" s="3" t="n">
+      <c r="AL32" s="86" t="n">
         <v>1327</v>
       </c>
-      <c r="AM32" s="3" t="n">
+      <c r="AM32" s="86" t="n">
         <v>1420</v>
       </c>
-      <c r="AN32" s="3" t="n">
+      <c r="AN32" s="86" t="n">
         <v>1798</v>
       </c>
+      <c r="AO32" s="90" t="n"/>
     </row>
     <row r="33" outlineLevel="1">
       <c r="B33" s="4" t="inlineStr">
@@ -60907,18 +60915,19 @@
       <c r="AJ33" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK33" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL33" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM33" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN33" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK33" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL33" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM33" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN33" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO33" s="90" t="n"/>
     </row>
     <row r="34" outlineLevel="1">
       <c r="B34" s="4" t="inlineStr">
@@ -61030,18 +61039,19 @@
       <c r="AJ34" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK34" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL34" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM34" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN34" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK34" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL34" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM34" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN34" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO34" s="90" t="n"/>
     </row>
     <row r="35" outlineLevel="1">
       <c r="B35" s="4" t="inlineStr">
@@ -61153,18 +61163,19 @@
       <c r="AJ35" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN35" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK35" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL35" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM35" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN35" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO35" s="90" t="n"/>
     </row>
     <row r="36" outlineLevel="1">
       <c r="B36" s="4" t="inlineStr">
@@ -61276,18 +61287,19 @@
       <c r="AJ36" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK36" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL36" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM36" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN36" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK36" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL36" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM36" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN36" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO36" s="90" t="n"/>
     </row>
     <row r="37" outlineLevel="1">
       <c r="B37" s="4" t="inlineStr">
@@ -61399,18 +61411,19 @@
       <c r="AJ37" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK37" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL37" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM37" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN37" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK37" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL37" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM37" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN37" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO37" s="90" t="n"/>
     </row>
     <row r="38" outlineLevel="1">
       <c r="B38" s="4" t="inlineStr">
@@ -61522,18 +61535,19 @@
       <c r="AJ38" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK38" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL38" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM38" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN38" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK38" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL38" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM38" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN38" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO38" s="90" t="n"/>
     </row>
     <row r="39" outlineLevel="1">
       <c r="B39" s="4" t="inlineStr">
@@ -61645,18 +61659,19 @@
       <c r="AJ39" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK39" s="3" t="n">
+      <c r="AK39" s="86" t="n">
         <v>39</v>
       </c>
-      <c r="AL39" s="3" t="n">
+      <c r="AL39" s="86" t="n">
         <v>59</v>
       </c>
-      <c r="AM39" s="3" t="n">
+      <c r="AM39" s="86" t="n">
         <v>52</v>
       </c>
-      <c r="AN39" s="3" t="n">
+      <c r="AN39" s="86" t="n">
         <v>23</v>
       </c>
+      <c r="AO39" s="90" t="n"/>
     </row>
     <row r="40" outlineLevel="1">
       <c r="B40" s="4" t="inlineStr">
@@ -61768,18 +61783,19 @@
       <c r="AJ40" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK40" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL40" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM40" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN40" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK40" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL40" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM40" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN40" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO40" s="90" t="n"/>
     </row>
     <row r="41" outlineLevel="1">
       <c r="B41" s="4" t="inlineStr">
@@ -61891,18 +61907,19 @@
       <c r="AJ41" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK41" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL41" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM41" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN41" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK41" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL41" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM41" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN41" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO41" s="90" t="n"/>
     </row>
     <row r="42" outlineLevel="1">
       <c r="B42" s="4" t="inlineStr">
@@ -62014,18 +62031,19 @@
       <c r="AJ42" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK42" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL42" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM42" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN42" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK42" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL42" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM42" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN42" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO42" s="90" t="n"/>
     </row>
     <row r="43" outlineLevel="1">
       <c r="B43" s="4" t="inlineStr">
@@ -62137,18 +62155,19 @@
       <c r="AJ43" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK43" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL43" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM43" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN43" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK43" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL43" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM43" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN43" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO43" s="90" t="n"/>
     </row>
     <row r="44" outlineLevel="1">
       <c r="B44" s="4" t="inlineStr">
@@ -62260,18 +62279,19 @@
       <c r="AJ44" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK44" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL44" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM44" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN44" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK44" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL44" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM44" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN44" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO44" s="90" t="n"/>
     </row>
     <row r="45" outlineLevel="1">
       <c r="B45" s="4" t="inlineStr">
@@ -62383,18 +62403,19 @@
       <c r="AJ45" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK45" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL45" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM45" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN45" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK45" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL45" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM45" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN45" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO45" s="90" t="n"/>
     </row>
     <row r="46" outlineLevel="1">
       <c r="B46" s="4" t="inlineStr">
@@ -62506,18 +62527,19 @@
       <c r="AJ46" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK46" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL46" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM46" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN46" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK46" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL46" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM46" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN46" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO46" s="90" t="n"/>
     </row>
     <row r="47" outlineLevel="1">
       <c r="B47" s="4" t="inlineStr">
@@ -62629,18 +62651,19 @@
       <c r="AJ47" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK47" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL47" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM47" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN47" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK47" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL47" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM47" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN47" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO47" s="90" t="n"/>
     </row>
     <row r="48" outlineLevel="1">
       <c r="B48" s="4" t="inlineStr">
@@ -62752,18 +62775,19 @@
       <c r="AJ48" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK48" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL48" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM48" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN48" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK48" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL48" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM48" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN48" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO48" s="90" t="n"/>
     </row>
     <row r="49" outlineLevel="1">
       <c r="B49" s="4" t="inlineStr">
@@ -62875,18 +62899,19 @@
       <c r="AJ49" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK49" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL49" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM49" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN49" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK49" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL49" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM49" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN49" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO49" s="90" t="n"/>
     </row>
     <row r="50" outlineLevel="1">
       <c r="B50" s="4" t="inlineStr">
@@ -62998,18 +63023,19 @@
       <c r="AJ50" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK50" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL50" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM50" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN50" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK50" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL50" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM50" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN50" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO50" s="90" t="n"/>
     </row>
     <row r="51" outlineLevel="1">
       <c r="B51" s="4" t="inlineStr">
@@ -63121,18 +63147,19 @@
       <c r="AJ51" s="86" t="n">
         <v>3812</v>
       </c>
-      <c r="AK51" s="3" t="n">
+      <c r="AK51" s="86" t="n">
         <v>4190</v>
       </c>
-      <c r="AL51" s="3" t="n">
+      <c r="AL51" s="86" t="n">
         <v>4038</v>
       </c>
-      <c r="AM51" s="3" t="n">
+      <c r="AM51" s="86" t="n">
         <v>4328</v>
       </c>
-      <c r="AN51" s="3" t="n">
+      <c r="AN51" s="86" t="n">
         <v>4762</v>
       </c>
+      <c r="AO51" s="90" t="n"/>
     </row>
     <row r="52" outlineLevel="1">
       <c r="B52" s="4" t="inlineStr">
@@ -63244,18 +63271,19 @@
       <c r="AJ52" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK52" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL52" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM52" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN52" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK52" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL52" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM52" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN52" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO52" s="90" t="n"/>
     </row>
     <row r="53" outlineLevel="1">
       <c r="B53" s="4" t="inlineStr">
@@ -63367,18 +63395,19 @@
       <c r="AJ53" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK53" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL53" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM53" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN53" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK53" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL53" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM53" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN53" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO53" s="90" t="n"/>
     </row>
     <row r="54" outlineLevel="1">
       <c r="B54" s="4" t="inlineStr">
@@ -63490,18 +63519,19 @@
       <c r="AJ54" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK54" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL54" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM54" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN54" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK54" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL54" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM54" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN54" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO54" s="90" t="n"/>
     </row>
     <row r="55" outlineLevel="1">
       <c r="B55" s="4" t="inlineStr">
@@ -63613,18 +63643,19 @@
       <c r="AJ55" s="86" t="n">
         <v>2334</v>
       </c>
-      <c r="AK55" s="3" t="n">
+      <c r="AK55" s="86" t="n">
         <v>2382</v>
       </c>
-      <c r="AL55" s="3" t="n">
+      <c r="AL55" s="86" t="n">
         <v>2359</v>
       </c>
-      <c r="AM55" s="3" t="n">
+      <c r="AM55" s="86" t="n">
         <v>2932</v>
       </c>
-      <c r="AN55" s="3" t="n">
+      <c r="AN55" s="86" t="n">
         <v>2650</v>
       </c>
+      <c r="AO55" s="90" t="n"/>
     </row>
     <row r="56" outlineLevel="1">
       <c r="B56" s="4" t="inlineStr">
@@ -63736,18 +63767,19 @@
       <c r="AJ56" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK56" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL56" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM56" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN56" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK56" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL56" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM56" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN56" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO56" s="90" t="n"/>
     </row>
     <row r="57" outlineLevel="1">
       <c r="B57" s="4" t="inlineStr">
@@ -63859,18 +63891,19 @@
       <c r="AJ57" s="86" t="n">
         <v>0</v>
       </c>
-      <c r="AK57" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL57" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM57" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN57" s="3" t="n">
+      <c r="AK57" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL57" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM57" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN57" s="86" t="n">
         <v>264</v>
       </c>
+      <c r="AO57" s="90" t="n"/>
     </row>
     <row r="58" ht="15" customHeight="1">
       <c r="B58" s="50" t="n"/>
@@ -64011,23 +64044,23 @@
         <f>IF(SUM(AJ16:AJ57)=0,"",SUM(AJ16:AJ57))</f>
         <v/>
       </c>
-      <c r="AK58" s="2">
+      <c r="AK58" s="88">
         <f>IF(SUM(AK16:AK57)=0,"",SUM(AK16:AK57))</f>
         <v/>
       </c>
-      <c r="AL58" s="2">
+      <c r="AL58" s="88">
         <f>IF(SUM(AL16:AL57)=0,"",SUM(AL16:AL57))</f>
         <v/>
       </c>
-      <c r="AM58" s="2">
+      <c r="AM58" s="88">
         <f>IF(SUM(AM16:AM57)=0,"",SUM(AM16:AM57))</f>
         <v/>
       </c>
-      <c r="AN58" s="2">
+      <c r="AN58" s="88">
         <f>IF(SUM(AN16:AN57)=0,"",SUM(AN16:AN57))</f>
         <v/>
       </c>
-      <c r="AO58" s="1">
+      <c r="AO58" s="87">
         <f>IF(SUM(AO16:AO57)=0,"",SUM(AO16:AO57))</f>
         <v/>
       </c>
@@ -64181,206 +64214,84 @@
       </c>
     </row>
     <row r="59">
-      <c r="D59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="E59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="F59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="H59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="I59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="J59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="K59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="L59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="M59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="N59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="O59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="P59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="R59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="S59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="T59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="U59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="V59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="W59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="X59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI59" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ59" s="90" t="n">
-        <v>0</v>
-      </c>
+      <c r="D59" s="90" t="n"/>
+      <c r="E59" s="90" t="n"/>
+      <c r="F59" s="90" t="n"/>
+      <c r="G59" s="90" t="n"/>
+      <c r="H59" s="90" t="n"/>
+      <c r="I59" s="90" t="n"/>
+      <c r="J59" s="90" t="n"/>
+      <c r="K59" s="90" t="n"/>
+      <c r="L59" s="90" t="n"/>
+      <c r="M59" s="90" t="n"/>
+      <c r="N59" s="90" t="n"/>
+      <c r="O59" s="90" t="n"/>
+      <c r="P59" s="90" t="n"/>
+      <c r="Q59" s="90" t="n"/>
+      <c r="R59" s="90" t="n"/>
+      <c r="S59" s="90" t="n"/>
+      <c r="T59" s="90" t="n"/>
+      <c r="U59" s="90" t="n"/>
+      <c r="V59" s="90" t="n"/>
+      <c r="W59" s="90" t="n"/>
+      <c r="X59" s="90" t="n"/>
+      <c r="Y59" s="90" t="n"/>
+      <c r="Z59" s="90" t="n"/>
+      <c r="AA59" s="90" t="n"/>
+      <c r="AB59" s="90" t="n"/>
+      <c r="AC59" s="90" t="n"/>
+      <c r="AD59" s="90" t="n"/>
+      <c r="AE59" s="90" t="n"/>
+      <c r="AF59" s="90" t="n"/>
+      <c r="AG59" s="90" t="n"/>
+      <c r="AH59" s="90" t="n"/>
+      <c r="AI59" s="90" t="n"/>
+      <c r="AJ59" s="90" t="n"/>
+      <c r="AK59" s="90" t="n"/>
+      <c r="AL59" s="90" t="n"/>
+      <c r="AM59" s="90" t="n"/>
+      <c r="AN59" s="90" t="n"/>
+      <c r="AO59" s="90" t="n"/>
     </row>
     <row r="60">
-      <c r="D60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="E60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="F60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="H60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="I60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="J60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="K60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="L60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="M60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="N60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="O60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="P60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="R60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="S60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="T60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="U60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="V60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="W60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="X60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI60" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ60" s="90" t="n">
-        <v>0</v>
-      </c>
+      <c r="D60" s="90" t="n"/>
+      <c r="E60" s="90" t="n"/>
+      <c r="F60" s="90" t="n"/>
+      <c r="G60" s="90" t="n"/>
+      <c r="H60" s="90" t="n"/>
+      <c r="I60" s="90" t="n"/>
+      <c r="J60" s="90" t="n"/>
+      <c r="K60" s="90" t="n"/>
+      <c r="L60" s="90" t="n"/>
+      <c r="M60" s="90" t="n"/>
+      <c r="N60" s="90" t="n"/>
+      <c r="O60" s="90" t="n"/>
+      <c r="P60" s="90" t="n"/>
+      <c r="Q60" s="90" t="n"/>
+      <c r="R60" s="90" t="n"/>
+      <c r="S60" s="90" t="n"/>
+      <c r="T60" s="90" t="n"/>
+      <c r="U60" s="90" t="n"/>
+      <c r="V60" s="90" t="n"/>
+      <c r="W60" s="90" t="n"/>
+      <c r="X60" s="90" t="n"/>
+      <c r="Y60" s="90" t="n"/>
+      <c r="Z60" s="90" t="n"/>
+      <c r="AA60" s="90" t="n"/>
+      <c r="AB60" s="90" t="n"/>
+      <c r="AC60" s="90" t="n"/>
+      <c r="AD60" s="90" t="n"/>
+      <c r="AE60" s="90" t="n"/>
+      <c r="AF60" s="90" t="n"/>
+      <c r="AG60" s="90" t="n"/>
+      <c r="AH60" s="90" t="n"/>
+      <c r="AI60" s="90" t="n"/>
+      <c r="AJ60" s="90" t="n"/>
+      <c r="AK60" s="90" t="n"/>
+      <c r="AL60" s="90" t="n"/>
+      <c r="AM60" s="90" t="n"/>
+      <c r="AN60" s="90" t="n"/>
+      <c r="AO60" s="90" t="n"/>
     </row>
     <row r="61" ht="26.25" customHeight="1">
       <c r="B61" s="11" t="inlineStr">
@@ -64388,105 +64299,44 @@
           <t>b) Processed Requests | Other types of Specialist Advice</t>
         </is>
       </c>
-      <c r="D61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="E61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="H61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="I61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="J61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="K61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="L61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="O61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="P61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="R61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="S61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="T61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="U61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="V61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="W61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="X61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI61" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ61" s="90" t="n">
-        <v>0</v>
-      </c>
+      <c r="D61" s="90" t="n"/>
+      <c r="E61" s="90" t="n"/>
+      <c r="F61" s="90" t="n"/>
+      <c r="G61" s="90" t="n"/>
+      <c r="H61" s="90" t="n"/>
+      <c r="I61" s="90" t="n"/>
+      <c r="J61" s="90" t="n"/>
+      <c r="K61" s="90" t="n"/>
+      <c r="L61" s="90" t="n"/>
+      <c r="M61" s="90" t="n"/>
+      <c r="N61" s="90" t="n"/>
+      <c r="O61" s="90" t="n"/>
+      <c r="P61" s="90" t="n"/>
+      <c r="Q61" s="90" t="n"/>
+      <c r="R61" s="90" t="n"/>
+      <c r="S61" s="90" t="n"/>
+      <c r="T61" s="90" t="n"/>
+      <c r="U61" s="90" t="n"/>
+      <c r="V61" s="90" t="n"/>
+      <c r="W61" s="90" t="n"/>
+      <c r="X61" s="90" t="n"/>
+      <c r="Y61" s="90" t="n"/>
+      <c r="Z61" s="90" t="n"/>
+      <c r="AA61" s="90" t="n"/>
+      <c r="AB61" s="90" t="n"/>
+      <c r="AC61" s="90" t="n"/>
+      <c r="AD61" s="90" t="n"/>
+      <c r="AE61" s="90" t="n"/>
+      <c r="AF61" s="90" t="n"/>
+      <c r="AG61" s="90" t="n"/>
+      <c r="AH61" s="90" t="n"/>
+      <c r="AI61" s="90" t="n"/>
+      <c r="AJ61" s="90" t="n"/>
+      <c r="AK61" s="90" t="n"/>
+      <c r="AL61" s="90" t="n"/>
+      <c r="AM61" s="90" t="n"/>
+      <c r="AN61" s="90" t="n"/>
+      <c r="AO61" s="90" t="n"/>
     </row>
     <row r="62" ht="30" customHeight="1">
       <c r="B62" s="15" t="inlineStr">
@@ -64494,206 +64344,84 @@
           <t>The number of Specialist Advice requests that have been received and responded to. This does not include those that are open or in need of redirection at source:</t>
         </is>
       </c>
-      <c r="D62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="E62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="F62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="H62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="I62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="J62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="K62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="L62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="M62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="N62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="O62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="P62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="R62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="S62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="T62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="U62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="V62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="W62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="X62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI62" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ62" s="90" t="n">
-        <v>0</v>
-      </c>
+      <c r="D62" s="90" t="n"/>
+      <c r="E62" s="90" t="n"/>
+      <c r="F62" s="90" t="n"/>
+      <c r="G62" s="90" t="n"/>
+      <c r="H62" s="90" t="n"/>
+      <c r="I62" s="90" t="n"/>
+      <c r="J62" s="90" t="n"/>
+      <c r="K62" s="90" t="n"/>
+      <c r="L62" s="90" t="n"/>
+      <c r="M62" s="90" t="n"/>
+      <c r="N62" s="90" t="n"/>
+      <c r="O62" s="90" t="n"/>
+      <c r="P62" s="90" t="n"/>
+      <c r="Q62" s="90" t="n"/>
+      <c r="R62" s="90" t="n"/>
+      <c r="S62" s="90" t="n"/>
+      <c r="T62" s="90" t="n"/>
+      <c r="U62" s="90" t="n"/>
+      <c r="V62" s="90" t="n"/>
+      <c r="W62" s="90" t="n"/>
+      <c r="X62" s="90" t="n"/>
+      <c r="Y62" s="90" t="n"/>
+      <c r="Z62" s="90" t="n"/>
+      <c r="AA62" s="90" t="n"/>
+      <c r="AB62" s="90" t="n"/>
+      <c r="AC62" s="90" t="n"/>
+      <c r="AD62" s="90" t="n"/>
+      <c r="AE62" s="90" t="n"/>
+      <c r="AF62" s="90" t="n"/>
+      <c r="AG62" s="90" t="n"/>
+      <c r="AH62" s="90" t="n"/>
+      <c r="AI62" s="90" t="n"/>
+      <c r="AJ62" s="90" t="n"/>
+      <c r="AK62" s="90" t="n"/>
+      <c r="AL62" s="90" t="n"/>
+      <c r="AM62" s="90" t="n"/>
+      <c r="AN62" s="90" t="n"/>
+      <c r="AO62" s="90" t="n"/>
     </row>
     <row r="63">
-      <c r="D63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="E63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="F63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="H63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="I63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="J63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="K63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="L63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="M63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="N63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="O63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="P63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="R63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="S63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="T63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="U63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="V63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="W63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="X63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI63" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ63" s="90" t="n">
-        <v>0</v>
-      </c>
+      <c r="D63" s="90" t="n"/>
+      <c r="E63" s="90" t="n"/>
+      <c r="F63" s="90" t="n"/>
+      <c r="G63" s="90" t="n"/>
+      <c r="H63" s="90" t="n"/>
+      <c r="I63" s="90" t="n"/>
+      <c r="J63" s="90" t="n"/>
+      <c r="K63" s="90" t="n"/>
+      <c r="L63" s="90" t="n"/>
+      <c r="M63" s="90" t="n"/>
+      <c r="N63" s="90" t="n"/>
+      <c r="O63" s="90" t="n"/>
+      <c r="P63" s="90" t="n"/>
+      <c r="Q63" s="90" t="n"/>
+      <c r="R63" s="90" t="n"/>
+      <c r="S63" s="90" t="n"/>
+      <c r="T63" s="90" t="n"/>
+      <c r="U63" s="90" t="n"/>
+      <c r="V63" s="90" t="n"/>
+      <c r="W63" s="90" t="n"/>
+      <c r="X63" s="90" t="n"/>
+      <c r="Y63" s="90" t="n"/>
+      <c r="Z63" s="90" t="n"/>
+      <c r="AA63" s="90" t="n"/>
+      <c r="AB63" s="90" t="n"/>
+      <c r="AC63" s="90" t="n"/>
+      <c r="AD63" s="90" t="n"/>
+      <c r="AE63" s="90" t="n"/>
+      <c r="AF63" s="90" t="n"/>
+      <c r="AG63" s="90" t="n"/>
+      <c r="AH63" s="90" t="n"/>
+      <c r="AI63" s="90" t="n"/>
+      <c r="AJ63" s="90" t="n"/>
+      <c r="AK63" s="90" t="n"/>
+      <c r="AL63" s="90" t="n"/>
+      <c r="AM63" s="90" t="n"/>
+      <c r="AN63" s="90" t="n"/>
+      <c r="AO63" s="90" t="n"/>
     </row>
     <row r="64" ht="15" customHeight="1">
       <c r="B64" s="61" t="inlineStr">
@@ -70240,23 +69968,23 @@
         <f>IF(SUM(AJ65:AJ106)=0,"",SUM(AJ65:AJ106))</f>
         <v/>
       </c>
-      <c r="AK107" s="88">
+      <c r="AK107" s="2">
         <f>IF(SUM(AK65:AK106)=0,"",SUM(AK65:AK106))</f>
         <v/>
       </c>
-      <c r="AL107" s="88">
+      <c r="AL107" s="2">
         <f>IF(SUM(AL65:AL106)=0,"",SUM(AL65:AL106))</f>
         <v/>
       </c>
-      <c r="AM107" s="88">
+      <c r="AM107" s="2">
         <f>IF(SUM(AM65:AM106)=0,"",SUM(AM65:AM106))</f>
         <v/>
       </c>
-      <c r="AN107" s="88">
+      <c r="AN107" s="2">
         <f>IF(SUM(AN65:AN106)=0,"",SUM(AN65:AN106))</f>
         <v/>
       </c>
-      <c r="AO107" s="87">
+      <c r="AO107" s="1">
         <f>IF(SUM(AO65:AO106)=0,"",SUM(AO65:AO106))</f>
         <v/>
       </c>
@@ -70411,110 +70139,39 @@
     </row>
     <row r="108" customFormat="1" s="56">
       <c r="C108" s="57" t="n"/>
-      <c r="D108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="E108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="F108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="H108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="I108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="J108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="K108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="L108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="M108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="N108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="O108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="P108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="R108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="S108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="T108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="U108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="V108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="W108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="X108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ108" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK108" s="90" t="n"/>
-      <c r="AL108" s="90" t="n"/>
-      <c r="AM108" s="90" t="n"/>
-      <c r="AN108" s="90" t="n"/>
-      <c r="AO108" s="90" t="n"/>
+      <c r="D108" s="90" t="n"/>
+      <c r="E108" s="90" t="n"/>
+      <c r="F108" s="90" t="n"/>
+      <c r="G108" s="90" t="n"/>
+      <c r="H108" s="90" t="n"/>
+      <c r="I108" s="90" t="n"/>
+      <c r="J108" s="90" t="n"/>
+      <c r="K108" s="90" t="n"/>
+      <c r="L108" s="90" t="n"/>
+      <c r="M108" s="90" t="n"/>
+      <c r="N108" s="90" t="n"/>
+      <c r="O108" s="90" t="n"/>
+      <c r="P108" s="90" t="n"/>
+      <c r="Q108" s="90" t="n"/>
+      <c r="R108" s="90" t="n"/>
+      <c r="S108" s="90" t="n"/>
+      <c r="T108" s="90" t="n"/>
+      <c r="U108" s="90" t="n"/>
+      <c r="V108" s="90" t="n"/>
+      <c r="W108" s="90" t="n"/>
+      <c r="X108" s="90" t="n"/>
+      <c r="Y108" s="90" t="n"/>
+      <c r="Z108" s="90" t="n"/>
+      <c r="AA108" s="90" t="n"/>
+      <c r="AB108" s="90" t="n"/>
+      <c r="AC108" s="90" t="n"/>
+      <c r="AD108" s="90" t="n"/>
+      <c r="AE108" s="90" t="n"/>
+      <c r="AF108" s="90" t="n"/>
+      <c r="AG108" s="90" t="n"/>
+      <c r="AH108" s="90" t="n"/>
+      <c r="AI108" s="90" t="n"/>
+      <c r="AJ108" s="90" t="n"/>
     </row>
     <row r="109" ht="20.25" customFormat="1" customHeight="1" s="56">
       <c r="B109" s="60" t="inlineStr">
@@ -70523,110 +70180,39 @@
         </is>
       </c>
       <c r="C109" s="57" t="n"/>
-      <c r="D109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="E109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="F109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="H109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="I109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="J109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="K109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="L109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="M109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="N109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="O109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="P109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="R109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="S109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="T109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="U109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="V109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="W109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="X109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ109" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK109" s="90" t="n"/>
-      <c r="AL109" s="90" t="n"/>
-      <c r="AM109" s="90" t="n"/>
-      <c r="AN109" s="90" t="n"/>
-      <c r="AO109" s="90" t="n"/>
+      <c r="D109" s="90" t="n"/>
+      <c r="E109" s="90" t="n"/>
+      <c r="F109" s="90" t="n"/>
+      <c r="G109" s="90" t="n"/>
+      <c r="H109" s="90" t="n"/>
+      <c r="I109" s="90" t="n"/>
+      <c r="J109" s="90" t="n"/>
+      <c r="K109" s="90" t="n"/>
+      <c r="L109" s="90" t="n"/>
+      <c r="M109" s="90" t="n"/>
+      <c r="N109" s="90" t="n"/>
+      <c r="O109" s="90" t="n"/>
+      <c r="P109" s="90" t="n"/>
+      <c r="Q109" s="90" t="n"/>
+      <c r="R109" s="90" t="n"/>
+      <c r="S109" s="90" t="n"/>
+      <c r="T109" s="90" t="n"/>
+      <c r="U109" s="90" t="n"/>
+      <c r="V109" s="90" t="n"/>
+      <c r="W109" s="90" t="n"/>
+      <c r="X109" s="90" t="n"/>
+      <c r="Y109" s="90" t="n"/>
+      <c r="Z109" s="90" t="n"/>
+      <c r="AA109" s="90" t="n"/>
+      <c r="AB109" s="90" t="n"/>
+      <c r="AC109" s="90" t="n"/>
+      <c r="AD109" s="90" t="n"/>
+      <c r="AE109" s="90" t="n"/>
+      <c r="AF109" s="90" t="n"/>
+      <c r="AG109" s="90" t="n"/>
+      <c r="AH109" s="90" t="n"/>
+      <c r="AI109" s="90" t="n"/>
+      <c r="AJ109" s="90" t="n"/>
     </row>
     <row r="110" ht="30" customFormat="1" customHeight="1" s="56">
       <c r="B110" s="59" t="inlineStr">
@@ -70635,217 +70221,75 @@
         </is>
       </c>
       <c r="C110" s="57" t="n"/>
-      <c r="D110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="E110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="F110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="H110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="I110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="J110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="K110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="L110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="M110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="N110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="O110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="P110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="R110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="S110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="T110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="U110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="V110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="W110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="X110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ110" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK110" s="90" t="n"/>
-      <c r="AL110" s="90" t="n"/>
-      <c r="AM110" s="90" t="n"/>
-      <c r="AN110" s="90" t="n"/>
-      <c r="AO110" s="90" t="n"/>
+      <c r="D110" s="90" t="n"/>
+      <c r="E110" s="90" t="n"/>
+      <c r="F110" s="90" t="n"/>
+      <c r="G110" s="90" t="n"/>
+      <c r="H110" s="90" t="n"/>
+      <c r="I110" s="90" t="n"/>
+      <c r="J110" s="90" t="n"/>
+      <c r="K110" s="90" t="n"/>
+      <c r="L110" s="90" t="n"/>
+      <c r="M110" s="90" t="n"/>
+      <c r="N110" s="90" t="n"/>
+      <c r="O110" s="90" t="n"/>
+      <c r="P110" s="90" t="n"/>
+      <c r="Q110" s="90" t="n"/>
+      <c r="R110" s="90" t="n"/>
+      <c r="S110" s="90" t="n"/>
+      <c r="T110" s="90" t="n"/>
+      <c r="U110" s="90" t="n"/>
+      <c r="V110" s="90" t="n"/>
+      <c r="W110" s="90" t="n"/>
+      <c r="X110" s="90" t="n"/>
+      <c r="Y110" s="90" t="n"/>
+      <c r="Z110" s="90" t="n"/>
+      <c r="AA110" s="90" t="n"/>
+      <c r="AB110" s="90" t="n"/>
+      <c r="AC110" s="90" t="n"/>
+      <c r="AD110" s="90" t="n"/>
+      <c r="AE110" s="90" t="n"/>
+      <c r="AF110" s="90" t="n"/>
+      <c r="AG110" s="90" t="n"/>
+      <c r="AH110" s="90" t="n"/>
+      <c r="AI110" s="90" t="n"/>
+      <c r="AJ110" s="90" t="n"/>
     </row>
     <row r="111" customFormat="1" s="56">
       <c r="C111" s="57" t="n"/>
-      <c r="D111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="E111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="F111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="H111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="I111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="J111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="K111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="L111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="M111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="N111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="O111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="P111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="R111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="S111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="T111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="U111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="V111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="W111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="X111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ111" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK111" s="90" t="n"/>
-      <c r="AL111" s="90" t="n"/>
-      <c r="AM111" s="90" t="n"/>
-      <c r="AN111" s="90" t="n"/>
-      <c r="AO111" s="90" t="n"/>
+      <c r="D111" s="90" t="n"/>
+      <c r="E111" s="90" t="n"/>
+      <c r="F111" s="90" t="n"/>
+      <c r="G111" s="90" t="n"/>
+      <c r="H111" s="90" t="n"/>
+      <c r="I111" s="90" t="n"/>
+      <c r="J111" s="90" t="n"/>
+      <c r="K111" s="90" t="n"/>
+      <c r="L111" s="90" t="n"/>
+      <c r="M111" s="90" t="n"/>
+      <c r="N111" s="90" t="n"/>
+      <c r="O111" s="90" t="n"/>
+      <c r="P111" s="90" t="n"/>
+      <c r="Q111" s="90" t="n"/>
+      <c r="R111" s="90" t="n"/>
+      <c r="S111" s="90" t="n"/>
+      <c r="T111" s="90" t="n"/>
+      <c r="U111" s="90" t="n"/>
+      <c r="V111" s="90" t="n"/>
+      <c r="W111" s="90" t="n"/>
+      <c r="X111" s="90" t="n"/>
+      <c r="Y111" s="90" t="n"/>
+      <c r="Z111" s="90" t="n"/>
+      <c r="AA111" s="90" t="n"/>
+      <c r="AB111" s="90" t="n"/>
+      <c r="AC111" s="90" t="n"/>
+      <c r="AD111" s="90" t="n"/>
+      <c r="AE111" s="90" t="n"/>
+      <c r="AF111" s="90" t="n"/>
+      <c r="AG111" s="90" t="n"/>
+      <c r="AH111" s="90" t="n"/>
+      <c r="AI111" s="90" t="n"/>
+      <c r="AJ111" s="90" t="n"/>
     </row>
     <row r="112" ht="15" customHeight="1">
       <c r="B112" s="61" t="inlineStr">
@@ -70890,160 +70334,159 @@
       </c>
       <c r="J112" s="93" t="inlineStr">
         <is>
+          <t>Oct-2022</t>
+        </is>
+      </c>
+      <c r="K112" s="93" t="inlineStr">
+        <is>
+          <t>Nov-2022</t>
+        </is>
+      </c>
+      <c r="L112" s="93" t="inlineStr">
+        <is>
+          <t>Dec-2022</t>
+        </is>
+      </c>
+      <c r="M112" s="93" t="inlineStr">
+        <is>
           <t>Jan-2023</t>
         </is>
       </c>
-      <c r="K112" s="93" t="inlineStr">
+      <c r="N112" s="93" t="inlineStr">
+        <is>
+          <t>Feb-2023</t>
+        </is>
+      </c>
+      <c r="O112" s="93" t="inlineStr">
+        <is>
+          <t>Mar-2023</t>
+        </is>
+      </c>
+      <c r="P112" s="93" t="inlineStr">
         <is>
           <t>Apr-2023</t>
         </is>
       </c>
-      <c r="L112" s="93" t="inlineStr">
+      <c r="Q112" s="93" t="inlineStr">
         <is>
           <t>May-2023</t>
         </is>
       </c>
-      <c r="M112" s="93" t="inlineStr">
+      <c r="R112" s="93" t="inlineStr">
         <is>
           <t>Jun-2023</t>
         </is>
       </c>
-      <c r="N112" s="93" t="inlineStr">
+      <c r="S112" s="93" t="inlineStr">
         <is>
           <t>Jul-2023</t>
         </is>
       </c>
-      <c r="O112" s="93" t="inlineStr">
+      <c r="T112" s="93" t="inlineStr">
         <is>
           <t>Aug-2023</t>
         </is>
       </c>
-      <c r="P112" s="93" t="inlineStr">
+      <c r="U112" s="93" t="inlineStr">
         <is>
           <t>Sep-2023</t>
         </is>
       </c>
-      <c r="Q112" s="93" t="inlineStr">
+      <c r="V112" s="93" t="inlineStr">
         <is>
           <t>Oct-2023</t>
         </is>
       </c>
-      <c r="R112" s="93" t="inlineStr">
+      <c r="W112" s="93" t="inlineStr">
         <is>
           <t>Nov-2023</t>
         </is>
       </c>
-      <c r="S112" s="93" t="inlineStr">
+      <c r="X112" s="93" t="inlineStr">
         <is>
           <t>Dec-2023</t>
         </is>
       </c>
-      <c r="T112" s="93" t="inlineStr">
+      <c r="Y112" s="93" t="inlineStr">
         <is>
           <t>Jan-2024</t>
         </is>
       </c>
-      <c r="U112" s="93" t="inlineStr">
+      <c r="Z112" s="93" t="inlineStr">
         <is>
           <t>Feb-2024</t>
         </is>
       </c>
-      <c r="V112" s="93" t="inlineStr">
+      <c r="AA112" s="93" t="inlineStr">
         <is>
           <t>Mar-2024</t>
         </is>
       </c>
-      <c r="W112" s="93" t="inlineStr">
+      <c r="AB112" s="93" t="inlineStr">
         <is>
           <t>Apr-2024</t>
         </is>
       </c>
-      <c r="X112" s="93" t="inlineStr">
+      <c r="AC112" s="93" t="inlineStr">
         <is>
           <t>May-2024</t>
         </is>
       </c>
-      <c r="Y112" s="93" t="inlineStr">
+      <c r="AD112" s="93" t="inlineStr">
         <is>
           <t>Jun-2024</t>
         </is>
       </c>
-      <c r="Z112" s="93" t="inlineStr">
+      <c r="AE112" s="93" t="inlineStr">
         <is>
           <t>Jul-2024</t>
         </is>
       </c>
-      <c r="AA112" s="93" t="inlineStr">
+      <c r="AF112" s="93" t="inlineStr">
         <is>
           <t>Aug-2024</t>
         </is>
       </c>
-      <c r="AB112" s="93" t="inlineStr">
+      <c r="AG112" s="93" t="inlineStr">
         <is>
           <t>Sep-2024</t>
         </is>
       </c>
-      <c r="AC112" s="93" t="inlineStr">
+      <c r="AH112" s="93" t="inlineStr">
         <is>
           <t>Oct-2024</t>
         </is>
       </c>
-      <c r="AD112" s="93" t="inlineStr">
+      <c r="AI112" s="93" t="inlineStr">
         <is>
           <t>Nov-2024</t>
         </is>
       </c>
-      <c r="AE112" s="93" t="inlineStr">
+      <c r="AJ112" s="93" t="inlineStr">
         <is>
           <t>Dec-2024</t>
         </is>
       </c>
-      <c r="AF112" s="93" t="inlineStr">
+      <c r="AK112" s="5" t="inlineStr">
         <is>
           <t>Jan-2025</t>
         </is>
       </c>
-      <c r="AG112" s="93" t="inlineStr">
+      <c r="AL112" s="5" t="inlineStr">
         <is>
           <t>Feb-2025</t>
         </is>
       </c>
-      <c r="AH112" s="93" t="inlineStr">
+      <c r="AM112" s="5" t="inlineStr">
         <is>
           <t>Mar-2025</t>
         </is>
       </c>
-      <c r="AI112" s="93" t="inlineStr">
+      <c r="AN112" s="5" t="inlineStr">
         <is>
           <t>Apr-2025</t>
         </is>
       </c>
-      <c r="AJ112" s="93" t="inlineStr">
-        <is>
-          <t>Dec-2024</t>
-        </is>
-      </c>
-      <c r="AK112" s="93" t="inlineStr">
-        <is>
-          <t>Jan-2025</t>
-        </is>
-      </c>
-      <c r="AL112" s="93" t="inlineStr">
-        <is>
-          <t>Feb-2025</t>
-        </is>
-      </c>
-      <c r="AM112" s="93" t="inlineStr">
-        <is>
-          <t>Mar-2025</t>
-        </is>
-      </c>
-      <c r="AN112" s="93" t="inlineStr">
-        <is>
-          <t>Apr-2025</t>
-        </is>
-      </c>
-      <c r="AO112" s="90" t="n"/>
     </row>
     <row r="113" outlineLevel="1">
       <c r="B113" s="4" t="inlineStr">
@@ -71153,21 +70596,20 @@
         <v>0</v>
       </c>
       <c r="AJ113" s="86" t="n">
-        <v>965</v>
-      </c>
-      <c r="AK113" s="86" t="n">
-        <v>1589</v>
-      </c>
-      <c r="AL113" s="86" t="n">
-        <v>1499</v>
-      </c>
-      <c r="AM113" s="86" t="n">
-        <v>1564</v>
-      </c>
-      <c r="AN113" s="86" t="n">
-        <v>1452</v>
-      </c>
-      <c r="AO113" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN113" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="114" outlineLevel="1">
       <c r="B114" s="4" t="inlineStr">
@@ -71277,21 +70719,20 @@
         <v>0</v>
       </c>
       <c r="AJ114" s="86" t="n">
-        <v>1095</v>
-      </c>
-      <c r="AK114" s="86" t="n">
-        <v>1188</v>
-      </c>
-      <c r="AL114" s="86" t="n">
-        <v>1231</v>
-      </c>
-      <c r="AM114" s="86" t="n">
-        <v>1387</v>
-      </c>
-      <c r="AN114" s="86" t="n">
-        <v>939</v>
-      </c>
-      <c r="AO114" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN114" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="115" outlineLevel="1">
       <c r="B115" s="4" t="inlineStr">
@@ -71401,21 +70842,20 @@
         <v>0</v>
       </c>
       <c r="AJ115" s="86" t="n">
-        <v>1534</v>
-      </c>
-      <c r="AK115" s="86" t="n">
-        <v>1957</v>
-      </c>
-      <c r="AL115" s="86" t="n">
-        <v>1873</v>
-      </c>
-      <c r="AM115" s="86" t="n">
-        <v>1901</v>
-      </c>
-      <c r="AN115" s="86" t="n">
-        <v>1911</v>
-      </c>
-      <c r="AO115" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN115" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="116" outlineLevel="1">
       <c r="B116" s="4" t="inlineStr">
@@ -71525,21 +70965,20 @@
         <v>0</v>
       </c>
       <c r="AJ116" s="86" t="n">
-        <v>2097</v>
-      </c>
-      <c r="AK116" s="86" t="n">
-        <v>2539</v>
-      </c>
-      <c r="AL116" s="86" t="n">
-        <v>2539</v>
-      </c>
-      <c r="AM116" s="86" t="n">
-        <v>2713</v>
-      </c>
-      <c r="AN116" s="86" t="n">
-        <v>2215</v>
-      </c>
-      <c r="AO116" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN116" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="117" outlineLevel="1">
       <c r="B117" s="4" t="inlineStr">
@@ -71649,21 +71088,20 @@
         <v>0</v>
       </c>
       <c r="AJ117" s="86" t="n">
-        <v>885</v>
-      </c>
-      <c r="AK117" s="86" t="n">
-        <v>923</v>
-      </c>
-      <c r="AL117" s="86" t="n">
-        <v>970</v>
-      </c>
-      <c r="AM117" s="86" t="n">
-        <v>967</v>
-      </c>
-      <c r="AN117" s="86" t="n">
-        <v>722</v>
-      </c>
-      <c r="AO117" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN117" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="118" outlineLevel="1">
       <c r="B118" s="4" t="inlineStr">
@@ -71773,21 +71211,20 @@
         <v>0</v>
       </c>
       <c r="AJ118" s="86" t="n">
-        <v>2711</v>
-      </c>
-      <c r="AK118" s="86" t="n">
-        <v>2489</v>
-      </c>
-      <c r="AL118" s="86" t="n">
-        <v>3046</v>
-      </c>
-      <c r="AM118" s="86" t="n">
-        <v>3466</v>
-      </c>
-      <c r="AN118" s="86" t="n">
-        <v>2935</v>
-      </c>
-      <c r="AO118" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN118" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="119" outlineLevel="1">
       <c r="B119" s="4" t="inlineStr">
@@ -71897,21 +71334,20 @@
         <v>0</v>
       </c>
       <c r="AJ119" s="86" t="n">
-        <v>897</v>
-      </c>
-      <c r="AK119" s="86" t="n">
-        <v>1263</v>
-      </c>
-      <c r="AL119" s="86" t="n">
-        <v>1055</v>
-      </c>
-      <c r="AM119" s="86" t="n">
-        <v>1405</v>
-      </c>
-      <c r="AN119" s="86" t="n">
-        <v>1221</v>
-      </c>
-      <c r="AO119" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK119" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL119" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM119" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN119" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="120" outlineLevel="1">
       <c r="B120" s="4" t="inlineStr">
@@ -72021,21 +71457,20 @@
         <v>0</v>
       </c>
       <c r="AJ120" s="86" t="n">
-        <v>4059</v>
-      </c>
-      <c r="AK120" s="86" t="n">
-        <v>5128</v>
-      </c>
-      <c r="AL120" s="86" t="n">
-        <v>4899</v>
-      </c>
-      <c r="AM120" s="86" t="n">
-        <v>4645</v>
-      </c>
-      <c r="AN120" s="86" t="n">
-        <v>3093</v>
-      </c>
-      <c r="AO120" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN120" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="121" outlineLevel="1">
       <c r="B121" s="4" t="inlineStr">
@@ -72145,21 +71580,20 @@
         <v>0</v>
       </c>
       <c r="AJ121" s="86" t="n">
-        <v>1257</v>
-      </c>
-      <c r="AK121" s="86" t="n">
-        <v>1526</v>
-      </c>
-      <c r="AL121" s="86" t="n">
-        <v>1427</v>
-      </c>
-      <c r="AM121" s="86" t="n">
-        <v>1570</v>
-      </c>
-      <c r="AN121" s="86" t="n">
-        <v>1414</v>
-      </c>
-      <c r="AO121" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK121" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL121" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM121" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN121" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="122" outlineLevel="1">
       <c r="B122" s="4" t="inlineStr">
@@ -72269,21 +71703,20 @@
         <v>0</v>
       </c>
       <c r="AJ122" s="86" t="n">
-        <v>1111</v>
-      </c>
-      <c r="AK122" s="86" t="n">
-        <v>1302</v>
-      </c>
-      <c r="AL122" s="86" t="n">
-        <v>1448</v>
-      </c>
-      <c r="AM122" s="86" t="n">
-        <v>1699</v>
-      </c>
-      <c r="AN122" s="86" t="n">
-        <v>1209</v>
-      </c>
-      <c r="AO122" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN122" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="123" outlineLevel="1">
       <c r="B123" s="4" t="inlineStr">
@@ -72393,21 +71826,20 @@
         <v>0</v>
       </c>
       <c r="AJ123" s="86" t="n">
-        <v>935</v>
-      </c>
-      <c r="AK123" s="86" t="n">
-        <v>1049</v>
-      </c>
-      <c r="AL123" s="86" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AM123" s="86" t="n">
-        <v>1118</v>
-      </c>
-      <c r="AN123" s="86" t="n">
-        <v>823</v>
-      </c>
-      <c r="AO123" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN123" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" outlineLevel="1">
       <c r="B124" s="4" t="inlineStr">
@@ -72517,21 +71949,20 @@
         <v>0</v>
       </c>
       <c r="AJ124" s="86" t="n">
-        <v>1999</v>
-      </c>
-      <c r="AK124" s="86" t="n">
-        <v>2236</v>
-      </c>
-      <c r="AL124" s="86" t="n">
-        <v>2129</v>
-      </c>
-      <c r="AM124" s="86" t="n">
-        <v>2338</v>
-      </c>
-      <c r="AN124" s="86" t="n">
-        <v>2316</v>
-      </c>
-      <c r="AO124" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN124" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="125" outlineLevel="1">
       <c r="B125" s="4" t="inlineStr">
@@ -72641,21 +72072,20 @@
         <v>0</v>
       </c>
       <c r="AJ125" s="86" t="n">
-        <v>1194</v>
-      </c>
-      <c r="AK125" s="86" t="n">
-        <v>1309</v>
-      </c>
-      <c r="AL125" s="86" t="n">
-        <v>1208</v>
-      </c>
-      <c r="AM125" s="86" t="n">
-        <v>1242</v>
-      </c>
-      <c r="AN125" s="86" t="n">
-        <v>1108</v>
-      </c>
-      <c r="AO125" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN125" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="126" outlineLevel="1">
       <c r="B126" s="4" t="inlineStr">
@@ -72765,21 +72195,20 @@
         <v>0</v>
       </c>
       <c r="AJ126" s="86" t="n">
-        <v>1503</v>
-      </c>
-      <c r="AK126" s="86" t="n">
-        <v>1848</v>
-      </c>
-      <c r="AL126" s="86" t="n">
-        <v>2138</v>
-      </c>
-      <c r="AM126" s="86" t="n">
-        <v>2525</v>
-      </c>
-      <c r="AN126" s="86" t="n">
-        <v>2210</v>
-      </c>
-      <c r="AO126" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN126" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="127" outlineLevel="1">
       <c r="B127" s="4" t="inlineStr">
@@ -72889,21 +72318,20 @@
         <v>0</v>
       </c>
       <c r="AJ127" s="86" t="n">
-        <v>1576</v>
-      </c>
-      <c r="AK127" s="86" t="n">
-        <v>1526</v>
-      </c>
-      <c r="AL127" s="86" t="n">
-        <v>1477</v>
-      </c>
-      <c r="AM127" s="86" t="n">
-        <v>1524</v>
-      </c>
-      <c r="AN127" s="86" t="n">
-        <v>1511</v>
-      </c>
-      <c r="AO127" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN127" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="128" outlineLevel="1">
       <c r="B128" s="4" t="inlineStr">
@@ -73013,21 +72441,20 @@
         <v>0</v>
       </c>
       <c r="AJ128" s="86" t="n">
-        <v>7416</v>
-      </c>
-      <c r="AK128" s="86" t="n">
-        <v>8114</v>
-      </c>
-      <c r="AL128" s="86" t="n">
-        <v>8138</v>
-      </c>
-      <c r="AM128" s="86" t="n">
-        <v>9462</v>
-      </c>
-      <c r="AN128" s="86" t="n">
-        <v>7769</v>
-      </c>
-      <c r="AO128" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK128" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL128" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM128" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN128" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="129" outlineLevel="1">
       <c r="B129" s="4" t="inlineStr">
@@ -73062,96 +72489,95 @@
         <v>0</v>
       </c>
       <c r="K129" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="L129" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="M129" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="N129" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="O129" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="P129" s="86" t="n">
         <v>277</v>
       </c>
-      <c r="L129" s="86" t="n">
+      <c r="Q129" s="86" t="n">
         <v>349</v>
       </c>
-      <c r="M129" s="86" t="n">
+      <c r="R129" s="86" t="n">
         <v>343</v>
       </c>
-      <c r="N129" s="86" t="n">
+      <c r="S129" s="86" t="n">
         <v>349</v>
       </c>
-      <c r="O129" s="86" t="n">
+      <c r="T129" s="86" t="n">
         <v>335</v>
       </c>
-      <c r="P129" s="86" t="n">
+      <c r="U129" s="86" t="n">
         <v>371</v>
       </c>
-      <c r="Q129" s="86" t="n">
+      <c r="V129" s="86" t="n">
         <v>338</v>
       </c>
-      <c r="R129" s="86" t="n">
+      <c r="W129" s="86" t="n">
         <v>351</v>
       </c>
-      <c r="S129" s="86" t="n">
+      <c r="X129" s="86" t="n">
         <v>363</v>
       </c>
-      <c r="T129" s="86" t="n">
+      <c r="Y129" s="86" t="n">
         <v>396</v>
       </c>
-      <c r="U129" s="86" t="n">
+      <c r="Z129" s="86" t="n">
         <v>350</v>
       </c>
-      <c r="V129" s="86" t="n">
+      <c r="AA129" s="86" t="n">
         <v>301</v>
-      </c>
-      <c r="W129" s="86" t="n">
-        <v>1199</v>
-      </c>
-      <c r="X129" s="86" t="n">
-        <v>1391</v>
-      </c>
-      <c r="Y129" s="86" t="n">
-        <v>1214</v>
-      </c>
-      <c r="Z129" s="86" t="n">
-        <v>1228</v>
-      </c>
-      <c r="AA129" s="86" t="n">
-        <v>1035</v>
       </c>
       <c r="AB129" s="86" t="n">
         <v>1199</v>
       </c>
       <c r="AC129" s="86" t="n">
+        <v>1391</v>
+      </c>
+      <c r="AD129" s="86" t="n">
+        <v>1214</v>
+      </c>
+      <c r="AE129" s="86" t="n">
+        <v>1228</v>
+      </c>
+      <c r="AF129" s="86" t="n">
+        <v>1035</v>
+      </c>
+      <c r="AG129" s="86" t="n">
+        <v>1199</v>
+      </c>
+      <c r="AH129" s="86" t="n">
         <v>1361</v>
       </c>
-      <c r="AD129" s="86" t="n">
+      <c r="AI129" s="86" t="n">
         <v>1235</v>
       </c>
-      <c r="AE129" s="86" t="n">
+      <c r="AJ129" s="86" t="n">
         <v>1170</v>
       </c>
-      <c r="AF129" s="86" t="n">
+      <c r="AK129" s="3" t="n">
         <v>1342</v>
       </c>
-      <c r="AG129" s="86" t="n">
+      <c r="AL129" s="3" t="n">
         <v>1327</v>
       </c>
-      <c r="AH129" s="86" t="n">
+      <c r="AM129" s="3" t="n">
         <v>1420</v>
       </c>
-      <c r="AI129" s="86" t="n">
+      <c r="AN129" s="3" t="n">
         <v>1798</v>
       </c>
-      <c r="AJ129" s="86" t="n">
-        <v>2868</v>
-      </c>
-      <c r="AK129" s="86" t="n">
-        <v>2709</v>
-      </c>
-      <c r="AL129" s="86" t="n">
-        <v>3133</v>
-      </c>
-      <c r="AM129" s="86" t="n">
-        <v>3011</v>
-      </c>
-      <c r="AN129" s="86" t="n">
-        <v>2817</v>
-      </c>
-      <c r="AO129" s="90" t="n"/>
     </row>
     <row r="130" outlineLevel="1">
       <c r="B130" s="4" t="inlineStr">
@@ -73261,21 +72687,20 @@
         <v>0</v>
       </c>
       <c r="AJ130" s="86" t="n">
-        <v>1367</v>
-      </c>
-      <c r="AK130" s="86" t="n">
-        <v>1501</v>
-      </c>
-      <c r="AL130" s="86" t="n">
-        <v>1625</v>
-      </c>
-      <c r="AM130" s="86" t="n">
-        <v>1629</v>
-      </c>
-      <c r="AN130" s="86" t="n">
-        <v>1401</v>
-      </c>
-      <c r="AO130" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN130" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="131" outlineLevel="1">
       <c r="B131" s="4" t="inlineStr">
@@ -73385,21 +72810,20 @@
         <v>0</v>
       </c>
       <c r="AJ131" s="86" t="n">
-        <v>1412</v>
-      </c>
-      <c r="AK131" s="86" t="n">
-        <v>1487</v>
-      </c>
-      <c r="AL131" s="86" t="n">
-        <v>1469</v>
-      </c>
-      <c r="AM131" s="86" t="n">
-        <v>1678</v>
-      </c>
-      <c r="AN131" s="86" t="n">
-        <v>1519</v>
-      </c>
-      <c r="AO131" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN131" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="132" outlineLevel="1">
       <c r="B132" s="4" t="inlineStr">
@@ -73509,21 +72933,20 @@
         <v>0</v>
       </c>
       <c r="AJ132" s="86" t="n">
-        <v>2822</v>
-      </c>
-      <c r="AK132" s="86" t="n">
-        <v>4200</v>
-      </c>
-      <c r="AL132" s="86" t="n">
-        <v>3401</v>
-      </c>
-      <c r="AM132" s="86" t="n">
-        <v>3892</v>
-      </c>
-      <c r="AN132" s="86" t="n">
-        <v>3487</v>
-      </c>
-      <c r="AO132" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN132" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="133" outlineLevel="1">
       <c r="B133" s="4" t="inlineStr">
@@ -73633,21 +73056,20 @@
         <v>0</v>
       </c>
       <c r="AJ133" s="86" t="n">
-        <v>1951</v>
-      </c>
-      <c r="AK133" s="86" t="n">
-        <v>2132</v>
-      </c>
-      <c r="AL133" s="86" t="n">
-        <v>2051</v>
-      </c>
-      <c r="AM133" s="86" t="n">
-        <v>2305</v>
-      </c>
-      <c r="AN133" s="86" t="n">
-        <v>2118</v>
-      </c>
-      <c r="AO133" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN133" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="134" outlineLevel="1">
       <c r="B134" s="4" t="inlineStr">
@@ -73757,21 +73179,20 @@
         <v>0</v>
       </c>
       <c r="AJ134" s="86" t="n">
-        <v>2350</v>
-      </c>
-      <c r="AK134" s="86" t="n">
-        <v>2382</v>
-      </c>
-      <c r="AL134" s="86" t="n">
-        <v>2239</v>
-      </c>
-      <c r="AM134" s="86" t="n">
-        <v>2409</v>
-      </c>
-      <c r="AN134" s="86" t="n">
-        <v>2157</v>
-      </c>
-      <c r="AO134" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN134" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="135" outlineLevel="1">
       <c r="B135" s="4" t="inlineStr">
@@ -73881,21 +73302,20 @@
         <v>0</v>
       </c>
       <c r="AJ135" s="86" t="n">
-        <v>1888</v>
-      </c>
-      <c r="AK135" s="86" t="n">
-        <v>2538</v>
-      </c>
-      <c r="AL135" s="86" t="n">
-        <v>2326</v>
-      </c>
-      <c r="AM135" s="86" t="n">
-        <v>2343</v>
-      </c>
-      <c r="AN135" s="86" t="n">
-        <v>1527</v>
-      </c>
-      <c r="AO135" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN135" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="136" outlineLevel="1">
       <c r="B136" s="4" t="inlineStr">
@@ -73927,99 +73347,98 @@
         <v>1</v>
       </c>
       <c r="J136" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="K136" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="L136" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="M136" s="86" t="n">
         <v>8</v>
       </c>
-      <c r="K136" s="86" t="n">
+      <c r="N136" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="O136" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="P136" s="86" t="n">
         <v>9</v>
       </c>
-      <c r="L136" s="86" t="n">
+      <c r="Q136" s="86" t="n">
         <v>15</v>
       </c>
-      <c r="M136" s="86" t="n">
+      <c r="R136" s="86" t="n">
         <v>17</v>
       </c>
-      <c r="N136" s="86" t="n">
+      <c r="S136" s="86" t="n">
         <v>9</v>
       </c>
-      <c r="O136" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="P136" s="86" t="n">
+      <c r="T136" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="U136" s="86" t="n">
         <v>4</v>
       </c>
-      <c r="Q136" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="R136" s="86" t="n">
+      <c r="V136" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="W136" s="86" t="n">
         <v>23</v>
       </c>
-      <c r="S136" s="86" t="n">
+      <c r="X136" s="86" t="n">
         <v>14</v>
       </c>
-      <c r="T136" s="86" t="n">
+      <c r="Y136" s="86" t="n">
         <v>29</v>
       </c>
-      <c r="U136" s="86" t="n">
+      <c r="Z136" s="86" t="n">
         <v>10</v>
       </c>
-      <c r="V136" s="86" t="n">
+      <c r="AA136" s="86" t="n">
         <v>33</v>
       </c>
-      <c r="W136" s="86" t="n">
+      <c r="AB136" s="86" t="n">
         <v>7</v>
       </c>
-      <c r="X136" s="86" t="n">
+      <c r="AC136" s="86" t="n">
         <v>23</v>
       </c>
-      <c r="Y136" s="86" t="n">
+      <c r="AD136" s="86" t="n">
         <v>35</v>
       </c>
-      <c r="Z136" s="86" t="n">
+      <c r="AE136" s="86" t="n">
         <v>9</v>
-      </c>
-      <c r="AA136" s="86" t="n">
-        <v>17</v>
-      </c>
-      <c r="AB136" s="86" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC136" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD136" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE136" s="86" t="n">
-        <v>0</v>
       </c>
       <c r="AF136" s="86" t="n">
         <v>17</v>
       </c>
       <c r="AG136" s="86" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH136" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI136" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ136" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK136" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="AL136" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AH136" s="86" t="n">
+      <c r="AM136" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="AI136" s="86" t="n">
+      <c r="AN136" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="AJ136" s="86" t="n">
-        <v>898</v>
-      </c>
-      <c r="AK136" s="86" t="n">
-        <v>1365</v>
-      </c>
-      <c r="AL136" s="86" t="n">
-        <v>1398</v>
-      </c>
-      <c r="AM136" s="86" t="n">
-        <v>1409</v>
-      </c>
-      <c r="AN136" s="86" t="n">
-        <v>1436</v>
-      </c>
-      <c r="AO136" s="90" t="n"/>
     </row>
     <row r="137" outlineLevel="1">
       <c r="B137" s="4" t="inlineStr">
@@ -74129,21 +73548,20 @@
         <v>0</v>
       </c>
       <c r="AJ137" s="86" t="n">
-        <v>1981</v>
-      </c>
-      <c r="AK137" s="86" t="n">
-        <v>2268</v>
-      </c>
-      <c r="AL137" s="86" t="n">
-        <v>1466</v>
-      </c>
-      <c r="AM137" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN137" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO137" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN137" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="138" outlineLevel="1">
       <c r="B138" s="4" t="inlineStr">
@@ -74253,21 +73671,20 @@
         <v>0</v>
       </c>
       <c r="AJ138" s="86" t="n">
-        <v>1466</v>
-      </c>
-      <c r="AK138" s="86" t="n">
-        <v>2061</v>
-      </c>
-      <c r="AL138" s="86" t="n">
-        <v>1811</v>
-      </c>
-      <c r="AM138" s="86" t="n">
-        <v>1931</v>
-      </c>
-      <c r="AN138" s="86" t="n">
-        <v>1508</v>
-      </c>
-      <c r="AO138" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN138" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="139" outlineLevel="1">
       <c r="B139" s="4" t="inlineStr">
@@ -74377,21 +73794,20 @@
         <v>0</v>
       </c>
       <c r="AJ139" s="86" t="n">
-        <v>1965</v>
-      </c>
-      <c r="AK139" s="86" t="n">
-        <v>2274</v>
-      </c>
-      <c r="AL139" s="86" t="n">
-        <v>2269</v>
-      </c>
-      <c r="AM139" s="86" t="n">
-        <v>2491</v>
-      </c>
-      <c r="AN139" s="86" t="n">
-        <v>1759</v>
-      </c>
-      <c r="AO139" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN139" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="140" outlineLevel="1">
       <c r="B140" s="4" t="inlineStr">
@@ -74501,21 +73917,20 @@
         <v>0</v>
       </c>
       <c r="AJ140" s="86" t="n">
-        <v>3206</v>
-      </c>
-      <c r="AK140" s="86" t="n">
-        <v>3872</v>
-      </c>
-      <c r="AL140" s="86" t="n">
-        <v>3526</v>
-      </c>
-      <c r="AM140" s="86" t="n">
-        <v>4414</v>
-      </c>
-      <c r="AN140" s="86" t="n">
-        <v>3705</v>
-      </c>
-      <c r="AO140" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN140" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="141" outlineLevel="1">
       <c r="B141" s="4" t="inlineStr">
@@ -74625,21 +74040,20 @@
         <v>0</v>
       </c>
       <c r="AJ141" s="86" t="n">
-        <v>5092</v>
-      </c>
-      <c r="AK141" s="86" t="n">
-        <v>6386</v>
-      </c>
-      <c r="AL141" s="86" t="n">
-        <v>5906</v>
-      </c>
-      <c r="AM141" s="86" t="n">
-        <v>6345</v>
-      </c>
-      <c r="AN141" s="86" t="n">
-        <v>5415</v>
-      </c>
-      <c r="AO141" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN141" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="142" outlineLevel="1">
       <c r="B142" s="4" t="inlineStr">
@@ -74749,21 +74163,20 @@
         <v>0</v>
       </c>
       <c r="AJ142" s="86" t="n">
-        <v>10207</v>
-      </c>
-      <c r="AK142" s="86" t="n">
-        <v>10564</v>
-      </c>
-      <c r="AL142" s="86" t="n">
-        <v>11038</v>
-      </c>
-      <c r="AM142" s="86" t="n">
-        <v>12175</v>
-      </c>
-      <c r="AN142" s="86" t="n">
-        <v>9358</v>
-      </c>
-      <c r="AO142" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN142" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="143" outlineLevel="1">
       <c r="B143" s="4" t="inlineStr">
@@ -74873,21 +74286,20 @@
         <v>0</v>
       </c>
       <c r="AJ143" s="86" t="n">
-        <v>1639</v>
-      </c>
-      <c r="AK143" s="86" t="n">
-        <v>1692</v>
-      </c>
-      <c r="AL143" s="86" t="n">
-        <v>1689</v>
-      </c>
-      <c r="AM143" s="86" t="n">
-        <v>1978</v>
-      </c>
-      <c r="AN143" s="86" t="n">
-        <v>1103</v>
-      </c>
-      <c r="AO143" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN143" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="144" outlineLevel="1">
       <c r="B144" s="4" t="inlineStr">
@@ -74997,21 +74409,20 @@
         <v>0</v>
       </c>
       <c r="AJ144" s="86" t="n">
-        <v>1669</v>
-      </c>
-      <c r="AK144" s="86" t="n">
-        <v>2026</v>
-      </c>
-      <c r="AL144" s="86" t="n">
-        <v>1843</v>
-      </c>
-      <c r="AM144" s="86" t="n">
-        <v>1547</v>
-      </c>
-      <c r="AN144" s="86" t="n">
-        <v>1465</v>
-      </c>
-      <c r="AO144" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK144" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL144" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM144" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN144" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="145" outlineLevel="1">
       <c r="B145" s="4" t="inlineStr">
@@ -75121,21 +74532,20 @@
         <v>0</v>
       </c>
       <c r="AJ145" s="86" t="n">
-        <v>545</v>
-      </c>
-      <c r="AK145" s="86" t="n">
-        <v>712</v>
-      </c>
-      <c r="AL145" s="86" t="n">
-        <v>651</v>
-      </c>
-      <c r="AM145" s="86" t="n">
-        <v>666</v>
-      </c>
-      <c r="AN145" s="86" t="n">
-        <v>443</v>
-      </c>
-      <c r="AO145" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN145" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="146" outlineLevel="1">
       <c r="B146" s="4" t="inlineStr">
@@ -75245,21 +74655,20 @@
         <v>0</v>
       </c>
       <c r="AJ146" s="86" t="n">
-        <v>787</v>
-      </c>
-      <c r="AK146" s="86" t="n">
-        <v>741</v>
-      </c>
-      <c r="AL146" s="86" t="n">
-        <v>931</v>
-      </c>
-      <c r="AM146" s="86" t="n">
-        <v>1431</v>
-      </c>
-      <c r="AN146" s="86" t="n">
-        <v>1170</v>
-      </c>
-      <c r="AO146" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN146" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="147" outlineLevel="1">
       <c r="B147" s="4" t="inlineStr">
@@ -75369,21 +74778,20 @@
         <v>0</v>
       </c>
       <c r="AJ147" s="86" t="n">
-        <v>3071</v>
-      </c>
-      <c r="AK147" s="86" t="n">
-        <v>3695</v>
-      </c>
-      <c r="AL147" s="86" t="n">
-        <v>3535</v>
-      </c>
-      <c r="AM147" s="86" t="n">
-        <v>4121</v>
-      </c>
-      <c r="AN147" s="86" t="n">
-        <v>3842</v>
-      </c>
-      <c r="AO147" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN147" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="148" outlineLevel="1">
       <c r="B148" s="4" t="inlineStr">
@@ -75418,96 +74826,95 @@
         <v>0</v>
       </c>
       <c r="K148" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="L148" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="M148" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="N148" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="O148" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="P148" s="86" t="n">
         <v>457</v>
       </c>
-      <c r="L148" s="86" t="n">
+      <c r="Q148" s="86" t="n">
         <v>529</v>
       </c>
-      <c r="M148" s="86" t="n">
+      <c r="R148" s="86" t="n">
         <v>569</v>
       </c>
-      <c r="N148" s="86" t="n">
+      <c r="S148" s="86" t="n">
         <v>508</v>
       </c>
-      <c r="O148" s="86" t="n">
+      <c r="T148" s="86" t="n">
         <v>559</v>
       </c>
-      <c r="P148" s="86" t="n">
+      <c r="U148" s="86" t="n">
         <v>490</v>
       </c>
-      <c r="Q148" s="86" t="n">
+      <c r="V148" s="86" t="n">
         <v>555</v>
       </c>
-      <c r="R148" s="86" t="n">
+      <c r="W148" s="86" t="n">
         <v>590</v>
       </c>
-      <c r="S148" s="86" t="n">
+      <c r="X148" s="86" t="n">
         <v>487</v>
       </c>
-      <c r="T148" s="86" t="n">
+      <c r="Y148" s="86" t="n">
         <v>580</v>
       </c>
-      <c r="U148" s="86" t="n">
+      <c r="Z148" s="86" t="n">
         <v>565</v>
       </c>
-      <c r="V148" s="86" t="n">
+      <c r="AA148" s="86" t="n">
         <v>542</v>
       </c>
-      <c r="W148" s="86" t="n">
+      <c r="AB148" s="86" t="n">
         <v>556</v>
       </c>
-      <c r="X148" s="86" t="n">
+      <c r="AC148" s="86" t="n">
         <v>635</v>
       </c>
-      <c r="Y148" s="86" t="n">
+      <c r="AD148" s="86" t="n">
         <v>609</v>
       </c>
-      <c r="Z148" s="86" t="n">
+      <c r="AE148" s="86" t="n">
         <v>776</v>
       </c>
-      <c r="AA148" s="86" t="n">
+      <c r="AF148" s="86" t="n">
         <v>642</v>
       </c>
-      <c r="AB148" s="86" t="n">
+      <c r="AG148" s="86" t="n">
         <v>636</v>
       </c>
-      <c r="AC148" s="86" t="n">
+      <c r="AH148" s="86" t="n">
         <v>727</v>
       </c>
-      <c r="AD148" s="86" t="n">
+      <c r="AI148" s="86" t="n">
         <v>582</v>
       </c>
-      <c r="AE148" s="86" t="n">
+      <c r="AJ148" s="86" t="n">
         <v>542</v>
       </c>
-      <c r="AF148" s="86" t="n">
+      <c r="AK148" s="3" t="n">
         <v>641</v>
       </c>
-      <c r="AG148" s="86" t="n">
+      <c r="AL148" s="3" t="n">
         <v>529</v>
       </c>
-      <c r="AH148" s="86" t="n">
+      <c r="AM148" s="3" t="n">
         <v>625</v>
       </c>
-      <c r="AI148" s="86" t="n">
+      <c r="AN148" s="3" t="n">
         <v>630</v>
       </c>
-      <c r="AJ148" s="86" t="n">
-        <v>2346</v>
-      </c>
-      <c r="AK148" s="86" t="n">
-        <v>2751</v>
-      </c>
-      <c r="AL148" s="86" t="n">
-        <v>2729</v>
-      </c>
-      <c r="AM148" s="86" t="n">
-        <v>3097</v>
-      </c>
-      <c r="AN148" s="86" t="n">
-        <v>2552</v>
-      </c>
-      <c r="AO148" s="90" t="n"/>
     </row>
     <row r="149" outlineLevel="1">
       <c r="B149" s="4" t="inlineStr">
@@ -75617,21 +75024,20 @@
         <v>0</v>
       </c>
       <c r="AJ149" s="86" t="n">
-        <v>4021</v>
-      </c>
-      <c r="AK149" s="86" t="n">
-        <v>5236</v>
-      </c>
-      <c r="AL149" s="86" t="n">
-        <v>5600</v>
-      </c>
-      <c r="AM149" s="86" t="n">
-        <v>5608</v>
-      </c>
-      <c r="AN149" s="86" t="n">
-        <v>3644</v>
-      </c>
-      <c r="AO149" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN149" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="150" outlineLevel="1">
       <c r="B150" s="4" t="inlineStr">
@@ -75741,21 +75147,20 @@
         <v>0</v>
       </c>
       <c r="AJ150" s="86" t="n">
-        <v>1216</v>
-      </c>
-      <c r="AK150" s="86" t="n">
-        <v>1650</v>
-      </c>
-      <c r="AL150" s="86" t="n">
-        <v>1520</v>
-      </c>
-      <c r="AM150" s="86" t="n">
-        <v>1655</v>
-      </c>
-      <c r="AN150" s="86" t="n">
-        <v>1232</v>
-      </c>
-      <c r="AO150" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN150" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="151" outlineLevel="1">
       <c r="B151" s="4" t="inlineStr">
@@ -75865,21 +75270,20 @@
         <v>0</v>
       </c>
       <c r="AJ151" s="86" t="n">
-        <v>2165</v>
-      </c>
-      <c r="AK151" s="86" t="n">
-        <v>2938</v>
-      </c>
-      <c r="AL151" s="86" t="n">
-        <v>2562</v>
-      </c>
-      <c r="AM151" s="86" t="n">
-        <v>2289</v>
-      </c>
-      <c r="AN151" s="86" t="n">
-        <v>1915</v>
-      </c>
-      <c r="AO151" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN151" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="152" outlineLevel="1">
       <c r="B152" s="4" t="inlineStr">
@@ -75914,96 +75318,95 @@
         <v>0</v>
       </c>
       <c r="K152" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="L152" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="M152" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="N152" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="O152" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="P152" s="86" t="n">
         <v>299</v>
       </c>
-      <c r="L152" s="86" t="n">
+      <c r="Q152" s="86" t="n">
         <v>229</v>
       </c>
-      <c r="M152" s="86" t="n">
+      <c r="R152" s="86" t="n">
         <v>423</v>
       </c>
-      <c r="N152" s="86" t="n">
+      <c r="S152" s="86" t="n">
         <v>331</v>
       </c>
-      <c r="O152" s="86" t="n">
+      <c r="T152" s="86" t="n">
         <v>326</v>
       </c>
-      <c r="P152" s="86" t="n">
+      <c r="U152" s="86" t="n">
         <v>261</v>
       </c>
-      <c r="Q152" s="86" t="n">
+      <c r="V152" s="86" t="n">
         <v>353</v>
       </c>
-      <c r="R152" s="86" t="n">
+      <c r="W152" s="86" t="n">
         <v>339</v>
       </c>
-      <c r="S152" s="86" t="n">
+      <c r="X152" s="86" t="n">
         <v>293</v>
       </c>
-      <c r="T152" s="86" t="n">
+      <c r="Y152" s="86" t="n">
         <v>437</v>
       </c>
-      <c r="U152" s="86" t="n">
+      <c r="Z152" s="86" t="n">
         <v>320</v>
       </c>
-      <c r="V152" s="86" t="n">
+      <c r="AA152" s="86" t="n">
         <v>384</v>
       </c>
-      <c r="W152" s="86" t="n">
+      <c r="AB152" s="86" t="n">
         <v>341</v>
       </c>
-      <c r="X152" s="86" t="n">
+      <c r="AC152" s="86" t="n">
         <v>398</v>
       </c>
-      <c r="Y152" s="86" t="n">
+      <c r="AD152" s="86" t="n">
         <v>318</v>
       </c>
-      <c r="Z152" s="86" t="n">
+      <c r="AE152" s="86" t="n">
         <v>389</v>
       </c>
-      <c r="AA152" s="86" t="n">
+      <c r="AF152" s="86" t="n">
         <v>400</v>
       </c>
-      <c r="AB152" s="86" t="n">
+      <c r="AG152" s="86" t="n">
         <v>353</v>
       </c>
-      <c r="AC152" s="86" t="n">
+      <c r="AH152" s="86" t="n">
         <v>379</v>
       </c>
-      <c r="AD152" s="86" t="n">
+      <c r="AI152" s="86" t="n">
         <v>362</v>
       </c>
-      <c r="AE152" s="86" t="n">
+      <c r="AJ152" s="86" t="n">
         <v>287</v>
       </c>
-      <c r="AF152" s="86" t="n">
+      <c r="AK152" s="3" t="n">
         <v>321</v>
       </c>
-      <c r="AG152" s="86" t="n">
+      <c r="AL152" s="3" t="n">
         <v>306</v>
       </c>
-      <c r="AH152" s="86" t="n">
+      <c r="AM152" s="3" t="n">
         <v>403</v>
       </c>
-      <c r="AI152" s="86" t="n">
+      <c r="AN152" s="3" t="n">
         <v>337</v>
       </c>
-      <c r="AJ152" s="86" t="n">
-        <v>1841</v>
-      </c>
-      <c r="AK152" s="86" t="n">
-        <v>2182</v>
-      </c>
-      <c r="AL152" s="86" t="n">
-        <v>2222</v>
-      </c>
-      <c r="AM152" s="86" t="n">
-        <v>2165</v>
-      </c>
-      <c r="AN152" s="86" t="n">
-        <v>1610</v>
-      </c>
-      <c r="AO152" s="90" t="n"/>
     </row>
     <row r="153" outlineLevel="1">
       <c r="B153" s="4" t="inlineStr">
@@ -76113,21 +75516,20 @@
         <v>0</v>
       </c>
       <c r="AJ153" s="86" t="n">
-        <v>1213</v>
-      </c>
-      <c r="AK153" s="86" t="n">
-        <v>1412</v>
-      </c>
-      <c r="AL153" s="86" t="n">
-        <v>1134</v>
-      </c>
-      <c r="AM153" s="86" t="n">
-        <v>1208</v>
-      </c>
-      <c r="AN153" s="86" t="n">
-        <v>984</v>
-      </c>
-      <c r="AO153" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN153" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="154" outlineLevel="1">
       <c r="B154" s="4" t="inlineStr">
@@ -76237,21 +75639,20 @@
         <v>0</v>
       </c>
       <c r="AJ154" s="86" t="n">
-        <v>2986</v>
-      </c>
-      <c r="AK154" s="86" t="n">
-        <v>3659</v>
-      </c>
-      <c r="AL154" s="86" t="n">
-        <v>3518</v>
-      </c>
-      <c r="AM154" s="86" t="n">
-        <v>3708</v>
-      </c>
-      <c r="AN154" s="86" t="n">
-        <v>2858</v>
-      </c>
-      <c r="AO154" s="90" t="n"/>
+        <v>0</v>
+      </c>
+      <c r="AK154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN154" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="155" ht="15" customHeight="1">
       <c r="B155" s="50" t="n"/>

</xml_diff>